<commit_message>
update pemindahaan gantt chart
</commit_message>
<xml_diff>
--- a/panduan/Rev_Manualisasii1.xlsx
+++ b/panduan/Rev_Manualisasii1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\sim23\panduan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACCDDE5-96BF-4189-BC86-FF84B00E81A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63116FB1-E6B6-4D51-92B3-AA9E56F99E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ADB28F7E-1517-4DD0-AC52-7FAE16330C3D}"/>
+    <workbookView xWindow="7320" yWindow="-45" windowWidth="21600" windowHeight="11295" xr2:uid="{ADB28F7E-1517-4DD0-AC52-7FAE16330C3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset Original" sheetId="1" r:id="rId1"/>
@@ -950,7 +950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1236,13 +1236,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1254,9 +1320,6 @@
     <xf numFmtId="164" fontId="5" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1266,70 +1329,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5955,7 +5954,7 @@
   <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7247,7 +7246,7 @@
   <dimension ref="A1:AY78"/>
   <sheetViews>
     <sheetView topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:XFD64"/>
+      <selection activeCell="A62" sqref="A62:XFD62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7447,16 +7446,16 @@
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="N6" s="121" t="s">
+      <c r="N6" s="118" t="s">
         <v>89</v>
       </c>
-      <c r="O6" s="121"/>
-      <c r="P6" s="121"/>
-      <c r="Q6" s="121"/>
-      <c r="R6" s="121"/>
-      <c r="S6" s="121"/>
-      <c r="T6" s="121"/>
-      <c r="U6" s="121"/>
+      <c r="O6" s="118"/>
+      <c r="P6" s="118"/>
+      <c r="Q6" s="118"/>
+      <c r="R6" s="118"/>
+      <c r="S6" s="118"/>
+      <c r="T6" s="118"/>
+      <c r="U6" s="118"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="75">
@@ -7490,14 +7489,14 @@
       <c r="L7" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="121"/>
-      <c r="O7" s="121"/>
-      <c r="P7" s="121"/>
-      <c r="Q7" s="121"/>
-      <c r="R7" s="121"/>
-      <c r="S7" s="121"/>
-      <c r="T7" s="121"/>
-      <c r="U7" s="121"/>
+      <c r="N7" s="118"/>
+      <c r="O7" s="118"/>
+      <c r="P7" s="118"/>
+      <c r="Q7" s="118"/>
+      <c r="R7" s="118"/>
+      <c r="S7" s="118"/>
+      <c r="T7" s="118"/>
+      <c r="U7" s="118"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="75">
@@ -7531,14 +7530,14 @@
       <c r="L8" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="N8" s="121"/>
-      <c r="O8" s="121"/>
-      <c r="P8" s="121"/>
-      <c r="Q8" s="121"/>
-      <c r="R8" s="121"/>
-      <c r="S8" s="121"/>
-      <c r="T8" s="121"/>
-      <c r="U8" s="121"/>
+      <c r="N8" s="118"/>
+      <c r="O8" s="118"/>
+      <c r="P8" s="118"/>
+      <c r="Q8" s="118"/>
+      <c r="R8" s="118"/>
+      <c r="S8" s="118"/>
+      <c r="T8" s="118"/>
+      <c r="U8" s="118"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="75">
@@ -7566,14 +7565,14 @@
         <f t="shared" si="0"/>
         <v>209</v>
       </c>
-      <c r="N9" s="121"/>
-      <c r="O9" s="121"/>
-      <c r="P9" s="121"/>
-      <c r="Q9" s="121"/>
-      <c r="R9" s="121"/>
-      <c r="S9" s="121"/>
-      <c r="T9" s="121"/>
-      <c r="U9" s="121"/>
+      <c r="N9" s="118"/>
+      <c r="O9" s="118"/>
+      <c r="P9" s="118"/>
+      <c r="Q9" s="118"/>
+      <c r="R9" s="118"/>
+      <c r="S9" s="118"/>
+      <c r="T9" s="118"/>
+      <c r="U9" s="118"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="75">
@@ -7601,34 +7600,34 @@
         <f t="shared" si="0"/>
         <v>228</v>
       </c>
-      <c r="N10" s="121"/>
-      <c r="O10" s="121"/>
-      <c r="P10" s="121"/>
-      <c r="Q10" s="121"/>
-      <c r="R10" s="121"/>
-      <c r="S10" s="121"/>
-      <c r="T10" s="121"/>
-      <c r="U10" s="121"/>
+      <c r="N10" s="118"/>
+      <c r="O10" s="118"/>
+      <c r="P10" s="118"/>
+      <c r="Q10" s="118"/>
+      <c r="R10" s="118"/>
+      <c r="S10" s="118"/>
+      <c r="T10" s="118"/>
+      <c r="U10" s="118"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="N11" s="121"/>
-      <c r="O11" s="121"/>
-      <c r="P11" s="121"/>
-      <c r="Q11" s="121"/>
-      <c r="R11" s="121"/>
-      <c r="S11" s="121"/>
-      <c r="T11" s="121"/>
-      <c r="U11" s="121"/>
+      <c r="N11" s="118"/>
+      <c r="O11" s="118"/>
+      <c r="P11" s="118"/>
+      <c r="Q11" s="118"/>
+      <c r="R11" s="118"/>
+      <c r="S11" s="118"/>
+      <c r="T11" s="118"/>
+      <c r="U11" s="118"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N12" s="121"/>
-      <c r="O12" s="121"/>
-      <c r="P12" s="121"/>
-      <c r="Q12" s="121"/>
-      <c r="R12" s="121"/>
-      <c r="S12" s="121"/>
-      <c r="T12" s="121"/>
-      <c r="U12" s="121"/>
+      <c r="N12" s="118"/>
+      <c r="O12" s="118"/>
+      <c r="P12" s="118"/>
+      <c r="Q12" s="118"/>
+      <c r="R12" s="118"/>
+      <c r="S12" s="118"/>
+      <c r="T12" s="118"/>
+      <c r="U12" s="118"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
@@ -7641,18 +7640,18 @@
       <c r="D13" s="64"/>
       <c r="E13" s="64"/>
       <c r="F13" s="64"/>
-      <c r="G13" s="125" t="s">
+      <c r="G13" s="117" t="s">
         <v>45</v>
       </c>
       <c r="I13" s="40"/>
-      <c r="M13" s="137"/>
-      <c r="N13" s="134" t="s">
+      <c r="M13" s="112"/>
+      <c r="N13" s="132" t="s">
         <v>58</v>
       </c>
-      <c r="O13" s="134"/>
-      <c r="P13" s="134"/>
-      <c r="Q13" s="134"/>
-      <c r="R13" s="135"/>
+      <c r="O13" s="132"/>
+      <c r="P13" s="132"/>
+      <c r="Q13" s="132"/>
+      <c r="R13" s="133"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
@@ -7671,9 +7670,9 @@
       <c r="F14" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="125"/>
+      <c r="G14" s="117"/>
       <c r="I14" s="40"/>
-      <c r="M14" s="138"/>
+      <c r="M14" s="113"/>
       <c r="N14" s="37" t="s">
         <v>30</v>
       </c>
@@ -7750,7 +7749,7 @@
         <v>80</v>
       </c>
       <c r="B16" s="66">
-        <f t="shared" ref="B15:B23" si="6">($Q$15 * D3) / ($N$32 * $P$32)</f>
+        <f t="shared" ref="B16:B23" si="6">($Q$15 * D3) / ($N$32 * $P$32)</f>
         <v>107.61</v>
       </c>
       <c r="C16" s="66">
@@ -7802,14 +7801,14 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="M17" s="139"/>
-      <c r="N17" s="136" t="s">
+      <c r="M17" s="114"/>
+      <c r="N17" s="111" t="s">
         <v>59</v>
       </c>
-      <c r="O17" s="136"/>
-      <c r="P17" s="136"/>
-      <c r="Q17" s="136"/>
-      <c r="R17" s="136"/>
+      <c r="O17" s="111"/>
+      <c r="P17" s="111"/>
+      <c r="Q17" s="111"/>
+      <c r="R17" s="111"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="37" t="s">
@@ -7839,7 +7838,7 @@
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="M18" s="140"/>
+      <c r="M18" s="115"/>
       <c r="N18" s="37" t="s">
         <v>30</v>
       </c>
@@ -8030,7 +8029,7 @@
       <c r="D26" s="64"/>
       <c r="E26" s="64"/>
       <c r="F26" s="64"/>
-      <c r="G26" s="125" t="s">
+      <c r="G26" s="117" t="s">
         <v>6</v>
       </c>
       <c r="I26" s="62"/>
@@ -8052,7 +8051,7 @@
       <c r="F27" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="G27" s="125"/>
+      <c r="G27" s="117"/>
     </row>
     <row r="28" spans="1:18" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="s">
@@ -8406,38 +8405,38 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A39" s="116" t="s">
+      <c r="A39" s="138" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="141" t="s">
+      <c r="B39" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="141"/>
-      <c r="D39" s="141"/>
-      <c r="E39" s="141"/>
-      <c r="F39" s="141"/>
-      <c r="G39" s="141"/>
-      <c r="H39" s="141"/>
+      <c r="C39" s="116"/>
+      <c r="D39" s="116"/>
+      <c r="E39" s="116"/>
+      <c r="F39" s="116"/>
+      <c r="G39" s="116"/>
+      <c r="H39" s="116"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="116"/>
-      <c r="B40" s="122" t="s">
+      <c r="A40" s="138"/>
+      <c r="B40" s="120" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="123" t="s">
+      <c r="C40" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="124"/>
-      <c r="E40" s="124"/>
-      <c r="F40" s="124"/>
-      <c r="G40" s="124"/>
-      <c r="H40" s="125" t="s">
+      <c r="D40" s="122"/>
+      <c r="E40" s="122"/>
+      <c r="F40" s="122"/>
+      <c r="G40" s="122"/>
+      <c r="H40" s="117" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="117"/>
-      <c r="B41" s="122"/>
+      <c r="A41" s="125"/>
+      <c r="B41" s="120"/>
       <c r="C41" s="47" t="s">
         <v>72</v>
       </c>
@@ -8453,10 +8452,10 @@
       <c r="G41" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="H41" s="125"/>
+      <c r="H41" s="117"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="118">
+      <c r="A42" s="139">
         <v>44256</v>
       </c>
       <c r="B42" s="37">
@@ -8487,7 +8486,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="119"/>
+      <c r="A43" s="140"/>
       <c r="B43" s="37">
         <v>3</v>
       </c>
@@ -8517,19 +8516,19 @@
       <c r="I43" t="s">
         <v>108</v>
       </c>
-      <c r="N43" s="121" t="s">
+      <c r="N43" s="118" t="s">
         <v>89</v>
       </c>
-      <c r="O43" s="121"/>
-      <c r="P43" s="121"/>
-      <c r="Q43" s="121"/>
-      <c r="R43" s="121"/>
-      <c r="S43" s="121"/>
-      <c r="T43" s="121"/>
-      <c r="U43" s="121"/>
+      <c r="O43" s="118"/>
+      <c r="P43" s="118"/>
+      <c r="Q43" s="118"/>
+      <c r="R43" s="118"/>
+      <c r="S43" s="118"/>
+      <c r="T43" s="118"/>
+      <c r="U43" s="118"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="120"/>
+      <c r="A44" s="141"/>
       <c r="B44" s="37">
         <v>2</v>
       </c>
@@ -8556,17 +8555,17 @@
       <c r="H44" s="37">
         <v>13</v>
       </c>
-      <c r="N44" s="121"/>
-      <c r="O44" s="121"/>
-      <c r="P44" s="121"/>
-      <c r="Q44" s="121"/>
-      <c r="R44" s="121"/>
-      <c r="S44" s="121"/>
-      <c r="T44" s="121"/>
-      <c r="U44" s="121"/>
+      <c r="N44" s="118"/>
+      <c r="O44" s="118"/>
+      <c r="P44" s="118"/>
+      <c r="Q44" s="118"/>
+      <c r="R44" s="118"/>
+      <c r="S44" s="118"/>
+      <c r="T44" s="118"/>
+      <c r="U44" s="118"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="118">
+      <c r="A45" s="139">
         <v>44257</v>
       </c>
       <c r="B45" s="37">
@@ -8595,17 +8594,17 @@
       <c r="H45" s="37">
         <v>2</v>
       </c>
-      <c r="N45" s="121"/>
-      <c r="O45" s="121"/>
-      <c r="P45" s="121"/>
-      <c r="Q45" s="121"/>
-      <c r="R45" s="121"/>
-      <c r="S45" s="121"/>
-      <c r="T45" s="121"/>
-      <c r="U45" s="121"/>
+      <c r="N45" s="118"/>
+      <c r="O45" s="118"/>
+      <c r="P45" s="118"/>
+      <c r="Q45" s="118"/>
+      <c r="R45" s="118"/>
+      <c r="S45" s="118"/>
+      <c r="T45" s="118"/>
+      <c r="U45" s="118"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="119"/>
+      <c r="A46" s="140"/>
       <c r="B46" s="37">
         <v>6</v>
       </c>
@@ -8632,17 +8631,17 @@
       <c r="H46" s="37">
         <v>8</v>
       </c>
-      <c r="N46" s="121"/>
-      <c r="O46" s="121"/>
-      <c r="P46" s="121"/>
-      <c r="Q46" s="121"/>
-      <c r="R46" s="121"/>
-      <c r="S46" s="121"/>
-      <c r="T46" s="121"/>
-      <c r="U46" s="121"/>
+      <c r="N46" s="118"/>
+      <c r="O46" s="118"/>
+      <c r="P46" s="118"/>
+      <c r="Q46" s="118"/>
+      <c r="R46" s="118"/>
+      <c r="S46" s="118"/>
+      <c r="T46" s="118"/>
+      <c r="U46" s="118"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="120"/>
+      <c r="A47" s="141"/>
       <c r="B47" s="37">
         <v>5</v>
       </c>
@@ -8669,17 +8668,17 @@
       <c r="H47" s="37">
         <v>11</v>
       </c>
-      <c r="N47" s="121"/>
-      <c r="O47" s="121"/>
-      <c r="P47" s="121"/>
-      <c r="Q47" s="121"/>
-      <c r="R47" s="121"/>
-      <c r="S47" s="121"/>
-      <c r="T47" s="121"/>
-      <c r="U47" s="121"/>
+      <c r="N47" s="118"/>
+      <c r="O47" s="118"/>
+      <c r="P47" s="118"/>
+      <c r="Q47" s="118"/>
+      <c r="R47" s="118"/>
+      <c r="S47" s="118"/>
+      <c r="T47" s="118"/>
+      <c r="U47" s="118"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="118">
+      <c r="A48" s="139">
         <v>44258</v>
       </c>
       <c r="B48" s="37">
@@ -8708,17 +8707,17 @@
       <c r="H48" s="37">
         <v>8</v>
       </c>
-      <c r="N48" s="121"/>
-      <c r="O48" s="121"/>
-      <c r="P48" s="121"/>
-      <c r="Q48" s="121"/>
-      <c r="R48" s="121"/>
-      <c r="S48" s="121"/>
-      <c r="T48" s="121"/>
-      <c r="U48" s="121"/>
+      <c r="N48" s="118"/>
+      <c r="O48" s="118"/>
+      <c r="P48" s="118"/>
+      <c r="Q48" s="118"/>
+      <c r="R48" s="118"/>
+      <c r="S48" s="118"/>
+      <c r="T48" s="118"/>
+      <c r="U48" s="118"/>
     </row>
     <row r="49" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A49" s="119"/>
+      <c r="A49" s="140"/>
       <c r="B49" s="37">
         <v>7</v>
       </c>
@@ -8745,17 +8744,17 @@
       <c r="H49" s="37">
         <v>9</v>
       </c>
-      <c r="N49" s="121"/>
-      <c r="O49" s="121"/>
-      <c r="P49" s="121"/>
-      <c r="Q49" s="121"/>
-      <c r="R49" s="121"/>
-      <c r="S49" s="121"/>
-      <c r="T49" s="121"/>
-      <c r="U49" s="121"/>
+      <c r="N49" s="118"/>
+      <c r="O49" s="118"/>
+      <c r="P49" s="118"/>
+      <c r="Q49" s="118"/>
+      <c r="R49" s="118"/>
+      <c r="S49" s="118"/>
+      <c r="T49" s="118"/>
+      <c r="U49" s="118"/>
     </row>
     <row r="50" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A50" s="120"/>
+      <c r="A50" s="141"/>
       <c r="B50" s="37">
         <v>8</v>
       </c>
@@ -8784,106 +8783,106 @@
       </c>
     </row>
     <row r="54" spans="1:51" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B54" s="126" t="s">
+      <c r="B54" s="123" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="126"/>
-      <c r="D54" s="126"/>
-      <c r="E54" s="126"/>
-      <c r="F54" s="126"/>
-      <c r="G54" s="126"/>
-      <c r="H54" s="126"/>
-      <c r="I54" s="126"/>
-      <c r="J54" s="126"/>
-      <c r="K54" s="126"/>
-      <c r="L54" s="126"/>
-      <c r="M54" s="126"/>
-      <c r="N54" s="126"/>
-      <c r="O54" s="126"/>
+      <c r="C54" s="123"/>
+      <c r="D54" s="123"/>
+      <c r="E54" s="123"/>
+      <c r="F54" s="123"/>
+      <c r="G54" s="123"/>
+      <c r="H54" s="123"/>
+      <c r="I54" s="123"/>
+      <c r="J54" s="123"/>
+      <c r="K54" s="123"/>
+      <c r="L54" s="123"/>
+      <c r="M54" s="123"/>
+      <c r="N54" s="123"/>
+      <c r="O54" s="123"/>
     </row>
     <row r="56" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B56" s="71"/>
       <c r="C56" s="49"/>
     </row>
     <row r="57" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A57" s="114" t="s">
+      <c r="A57" s="136" t="s">
         <v>87</v>
       </c>
-      <c r="B57" s="127" t="s">
+      <c r="B57" s="124" t="s">
         <v>77</v>
       </c>
-      <c r="C57" s="123" t="s">
+      <c r="C57" s="121" t="s">
         <v>63</v>
       </c>
-      <c r="D57" s="124"/>
-      <c r="E57" s="124"/>
-      <c r="F57" s="124"/>
-      <c r="G57" s="131"/>
-      <c r="H57" s="123" t="s">
+      <c r="D57" s="122"/>
+      <c r="E57" s="122"/>
+      <c r="F57" s="122"/>
+      <c r="G57" s="129"/>
+      <c r="H57" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="I57" s="124"/>
-      <c r="J57" s="124"/>
-      <c r="K57" s="124"/>
-      <c r="L57" s="131"/>
-      <c r="M57" s="129" t="s">
+      <c r="I57" s="122"/>
+      <c r="J57" s="122"/>
+      <c r="K57" s="122"/>
+      <c r="L57" s="129"/>
+      <c r="M57" s="127" t="s">
         <v>62</v>
       </c>
-      <c r="N57" s="125" t="s">
+      <c r="N57" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="O57" s="132" t="s">
+      <c r="O57" s="130" t="s">
         <v>66</v>
       </c>
-      <c r="P57" s="132" t="s">
+      <c r="P57" s="130" t="s">
         <v>68</v>
       </c>
-      <c r="R57" s="112" t="s">
+      <c r="R57" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="S57" s="112" t="s">
+      <c r="S57" s="119" t="s">
         <v>99</v>
       </c>
-      <c r="T57" s="112" t="s">
+      <c r="T57" s="119" t="s">
         <v>101</v>
       </c>
-      <c r="U57" s="113" t="s">
+      <c r="U57" s="135" t="s">
         <v>102</v>
       </c>
-      <c r="V57" s="113"/>
-      <c r="W57" s="113"/>
-      <c r="X57" s="113"/>
-      <c r="Y57" s="113"/>
-      <c r="Z57" s="113"/>
-      <c r="AA57" s="113"/>
-      <c r="AB57" s="113"/>
-      <c r="AC57" s="113"/>
-      <c r="AD57" s="113"/>
-      <c r="AE57" s="113"/>
-      <c r="AF57" s="113"/>
-      <c r="AG57" s="113"/>
-      <c r="AH57" s="113"/>
-      <c r="AI57" s="113"/>
-      <c r="AJ57" s="113"/>
-      <c r="AK57" s="113"/>
-      <c r="AL57" s="113"/>
-      <c r="AM57" s="113"/>
-      <c r="AN57" s="113"/>
-      <c r="AO57" s="113"/>
-      <c r="AP57" s="113"/>
-      <c r="AQ57" s="113"/>
-      <c r="AR57" s="113"/>
-      <c r="AS57" s="113"/>
-      <c r="AT57" s="113"/>
-      <c r="AU57" s="113"/>
-      <c r="AV57" s="113"/>
-      <c r="AW57" s="113"/>
-      <c r="AX57" s="113"/>
-      <c r="AY57" s="113"/>
+      <c r="V57" s="135"/>
+      <c r="W57" s="135"/>
+      <c r="X57" s="135"/>
+      <c r="Y57" s="135"/>
+      <c r="Z57" s="135"/>
+      <c r="AA57" s="135"/>
+      <c r="AB57" s="135"/>
+      <c r="AC57" s="135"/>
+      <c r="AD57" s="135"/>
+      <c r="AE57" s="135"/>
+      <c r="AF57" s="135"/>
+      <c r="AG57" s="135"/>
+      <c r="AH57" s="135"/>
+      <c r="AI57" s="135"/>
+      <c r="AJ57" s="135"/>
+      <c r="AK57" s="135"/>
+      <c r="AL57" s="135"/>
+      <c r="AM57" s="135"/>
+      <c r="AN57" s="135"/>
+      <c r="AO57" s="135"/>
+      <c r="AP57" s="135"/>
+      <c r="AQ57" s="135"/>
+      <c r="AR57" s="135"/>
+      <c r="AS57" s="135"/>
+      <c r="AT57" s="135"/>
+      <c r="AU57" s="135"/>
+      <c r="AV57" s="135"/>
+      <c r="AW57" s="135"/>
+      <c r="AX57" s="135"/>
+      <c r="AY57" s="135"/>
     </row>
     <row r="58" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A58" s="115"/>
-      <c r="B58" s="117"/>
+      <c r="A58" s="137"/>
+      <c r="B58" s="125"/>
       <c r="C58" s="47" t="s">
         <v>72</v>
       </c>
@@ -8914,13 +8913,13 @@
       <c r="L58" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="M58" s="130"/>
-      <c r="N58" s="128"/>
-      <c r="O58" s="132"/>
-      <c r="P58" s="132"/>
-      <c r="R58" s="133"/>
-      <c r="S58" s="112"/>
-      <c r="T58" s="112"/>
+      <c r="M58" s="128"/>
+      <c r="N58" s="126"/>
+      <c r="O58" s="130"/>
+      <c r="P58" s="130"/>
+      <c r="R58" s="131"/>
+      <c r="S58" s="119"/>
+      <c r="T58" s="119"/>
       <c r="U58">
         <v>1</v>
       </c>
@@ -9728,19 +9727,19 @@
       </c>
     </row>
     <row r="71" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="111" t="s">
+      <c r="A71" s="134" t="s">
         <v>98</v>
       </c>
-      <c r="B71" s="111"/>
-      <c r="C71" s="111"/>
-      <c r="D71" s="111"/>
-      <c r="E71" s="111"/>
-      <c r="F71" s="111"/>
-      <c r="G71" s="111"/>
-      <c r="H71" s="111"/>
-      <c r="I71" s="111"/>
-      <c r="J71" s="111"/>
-      <c r="K71" s="111"/>
+      <c r="B71" s="134"/>
+      <c r="C71" s="134"/>
+      <c r="D71" s="134"/>
+      <c r="E71" s="134"/>
+      <c r="F71" s="134"/>
+      <c r="G71" s="134"/>
+      <c r="H71" s="134"/>
+      <c r="I71" s="134"/>
+      <c r="J71" s="134"/>
+      <c r="K71" s="134"/>
       <c r="M71">
         <f t="shared" ref="M71:M78" si="28">M60/960</f>
         <v>4.9250388816550923E-3</v>
@@ -9750,17 +9749,17 @@
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A72" s="111"/>
-      <c r="B72" s="111"/>
-      <c r="C72" s="111"/>
-      <c r="D72" s="111"/>
-      <c r="E72" s="111"/>
-      <c r="F72" s="111"/>
-      <c r="G72" s="111"/>
-      <c r="H72" s="111"/>
-      <c r="I72" s="111"/>
-      <c r="J72" s="111"/>
-      <c r="K72" s="111"/>
+      <c r="A72" s="134"/>
+      <c r="B72" s="134"/>
+      <c r="C72" s="134"/>
+      <c r="D72" s="134"/>
+      <c r="E72" s="134"/>
+      <c r="F72" s="134"/>
+      <c r="G72" s="134"/>
+      <c r="H72" s="134"/>
+      <c r="I72" s="134"/>
+      <c r="J72" s="134"/>
+      <c r="K72" s="134"/>
       <c r="M72">
         <f t="shared" si="28"/>
         <v>5.5056233723958341E-3</v>
@@ -9773,22 +9772,22 @@
       </c>
     </row>
     <row r="73" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="111"/>
-      <c r="B73" s="111"/>
-      <c r="C73" s="111"/>
-      <c r="D73" s="111"/>
-      <c r="E73" s="111"/>
-      <c r="F73" s="111"/>
-      <c r="G73" s="111"/>
-      <c r="H73" s="111"/>
-      <c r="I73" s="111"/>
-      <c r="J73" s="111"/>
-      <c r="K73" s="111"/>
+      <c r="A73" s="134"/>
+      <c r="B73" s="134"/>
+      <c r="C73" s="134"/>
+      <c r="D73" s="134"/>
+      <c r="E73" s="134"/>
+      <c r="F73" s="134"/>
+      <c r="G73" s="134"/>
+      <c r="H73" s="134"/>
+      <c r="I73" s="134"/>
+      <c r="J73" s="134"/>
+      <c r="K73" s="134"/>
       <c r="M73">
         <f t="shared" si="28"/>
         <v>4.6684932002314817E-3</v>
       </c>
-      <c r="P73" s="142">
+      <c r="P73">
         <v>725.12</v>
       </c>
       <c r="U73" t="s">
@@ -9796,17 +9795,17 @@
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A74" s="111"/>
-      <c r="B74" s="111"/>
-      <c r="C74" s="111"/>
-      <c r="D74" s="111"/>
-      <c r="E74" s="111"/>
-      <c r="F74" s="111"/>
-      <c r="G74" s="111"/>
-      <c r="H74" s="111"/>
-      <c r="I74" s="111"/>
-      <c r="J74" s="111"/>
-      <c r="K74" s="111"/>
+      <c r="A74" s="134"/>
+      <c r="B74" s="134"/>
+      <c r="C74" s="134"/>
+      <c r="D74" s="134"/>
+      <c r="E74" s="134"/>
+      <c r="F74" s="134"/>
+      <c r="G74" s="134"/>
+      <c r="H74" s="134"/>
+      <c r="I74" s="134"/>
+      <c r="J74" s="134"/>
+      <c r="K74" s="134"/>
       <c r="M74">
         <f t="shared" si="28"/>
         <v>2.57611400462963E-3</v>
@@ -9816,17 +9815,17 @@
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A75" s="111"/>
-      <c r="B75" s="111"/>
-      <c r="C75" s="111"/>
-      <c r="D75" s="111"/>
-      <c r="E75" s="111"/>
-      <c r="F75" s="111"/>
-      <c r="G75" s="111"/>
-      <c r="H75" s="111"/>
-      <c r="I75" s="111"/>
-      <c r="J75" s="111"/>
-      <c r="K75" s="111"/>
+      <c r="A75" s="134"/>
+      <c r="B75" s="134"/>
+      <c r="C75" s="134"/>
+      <c r="D75" s="134"/>
+      <c r="E75" s="134"/>
+      <c r="F75" s="134"/>
+      <c r="G75" s="134"/>
+      <c r="H75" s="134"/>
+      <c r="I75" s="134"/>
+      <c r="J75" s="134"/>
+      <c r="K75" s="134"/>
       <c r="M75">
         <f t="shared" si="28"/>
         <v>3.6468713831018522E-3</v>
@@ -9868,12 +9867,14 @@
     <sortCondition ref="G42:G50"/>
   </sortState>
   <mergeCells count="30">
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A71:K75"/>
+    <mergeCell ref="T57:T58"/>
+    <mergeCell ref="U57:AY57"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
     <mergeCell ref="N6:U12"/>
     <mergeCell ref="N43:U49"/>
     <mergeCell ref="S57:S58"/>
@@ -9890,14 +9891,12 @@
     <mergeCell ref="R57:R58"/>
     <mergeCell ref="N13:R13"/>
     <mergeCell ref="P57:P58"/>
-    <mergeCell ref="A71:K75"/>
-    <mergeCell ref="T57:T58"/>
-    <mergeCell ref="U57:AY57"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>